<commit_message>
Just kidding, this one is the final commit
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>Assertions</t>
   </si>
@@ -222,6 +222,18 @@
   </si>
   <si>
     <t>Long clicking removes favorites from list.  Changes status in database.</t>
+  </si>
+  <si>
+    <t>Random button</t>
+  </si>
+  <si>
+    <t>As a user, the app can suggest a restaurant for me</t>
+  </si>
+  <si>
+    <t>After clicking the "Surprise Me" button, a random restaurant is selected and presented to me</t>
+  </si>
+  <si>
+    <t>Clicked the button multiple times and it opened different restaurants.</t>
   </si>
 </sst>
 </file>
@@ -254,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,8 +297,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -331,11 +349,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -355,6 +388,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,9 +667,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F25"/>
+  <dimension ref="B2:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -815,6 +852,9 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="20" t="s">
+        <v>66</v>
+      </c>
       <c r="D17" t="s">
         <v>24</v>
       </c>
@@ -908,6 +948,22 @@
         <v>65</v>
       </c>
     </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>